<commit_message>
Gold standard mapping comparison
</commit_message>
<xml_diff>
--- a/Python/Data/Final/blood_pmbc.xlsx
+++ b/Python/Data/Final/blood_pmbc.xlsx
@@ -14,13 +14,14 @@
     <sheet name="Asctb_match_tree_crosswalk" sheetId="5" r:id="rId5"/>
     <sheet name="Az_cts_mismatch_final" sheetId="6" r:id="rId6"/>
     <sheet name="Asctb_cts_mismatch_final" sheetId="7" r:id="rId7"/>
+    <sheet name="Final_Matches" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="222">
   <si>
     <t>AZ.CT/ID</t>
   </si>
@@ -3093,4 +3094,257 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>